<commit_message>
Fix no move bug
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -227,6 +227,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">現在のゾーン内の家畜</t>
     </r>
@@ -246,6 +247,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">当前区域中的家畜</t>
     </r>
@@ -283,6 +285,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">現在のゾーン内の家畜</t>
     </r>
@@ -300,6 +303,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">を選択に追加します。</t>
     </r>
@@ -310,6 +314,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">将当前区域的家畜</t>
     </r>
@@ -327,6 +332,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">添加到您的选择中。</t>
     </r>
@@ -339,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -366,11 +372,6 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,10 +430,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -561,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -707,10 +704,10 @@
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -721,10 +718,10 @@
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -735,10 +732,10 @@
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>